<commit_message>
Actualización de main, cominzo de modelos ML
</commit_message>
<xml_diff>
--- a/data/ref/Microciclos.xlsx
+++ b/data/ref/Microciclos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532E7E0D-E806-486F-8F1E-8945205F3F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3637CD39-DC75-427A-98C4-3B668E33D53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D2A59680-2B68-43A7-A0B3-40444AC197F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="35">
   <si>
     <t>Fecha</t>
   </si>
@@ -138,13 +138,16 @@
   </si>
   <si>
     <t>Tipo_Dia</t>
+  </si>
+  <si>
+    <t>Pumas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -154,6 +157,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -179,9 +190,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6662318-5429-45BF-A116-92A73FB7B911}">
-  <dimension ref="A1:G130"/>
+  <dimension ref="A1:G145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="126" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="126" workbookViewId="0">
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2905,7 +2917,7 @@
         <v>21</v>
       </c>
       <c r="F128">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -2922,10 +2934,7 @@
         <v>29</v>
       </c>
       <c r="E129" t="s">
-        <v>21</v>
-      </c>
-      <c r="F129">
-        <v>-1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -2942,10 +2951,301 @@
         <v>29</v>
       </c>
       <c r="E130" t="s">
+        <v>21</v>
+      </c>
+      <c r="F130">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>45927</v>
+      </c>
+      <c r="B131">
+        <v>19</v>
+      </c>
+      <c r="C131" t="s">
+        <v>29</v>
+      </c>
+      <c r="D131" t="s">
+        <v>29</v>
+      </c>
+      <c r="E131" t="s">
         <v>16</v>
       </c>
-      <c r="G130" t="s">
+      <c r="G131" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>45928</v>
+      </c>
+      <c r="B132">
+        <v>19</v>
+      </c>
+      <c r="C132" t="s">
+        <v>29</v>
+      </c>
+      <c r="D132" t="s">
+        <v>29</v>
+      </c>
+      <c r="E132" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>45929</v>
+      </c>
+      <c r="B133">
+        <v>20</v>
+      </c>
+      <c r="C133" t="s">
+        <v>29</v>
+      </c>
+      <c r="D133" t="s">
+        <v>29</v>
+      </c>
+      <c r="E133" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>45930</v>
+      </c>
+      <c r="B134">
+        <v>20</v>
+      </c>
+      <c r="C134" t="s">
+        <v>29</v>
+      </c>
+      <c r="D134" t="s">
+        <v>29</v>
+      </c>
+      <c r="E134" t="s">
+        <v>21</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>45931</v>
+      </c>
+      <c r="B135">
+        <v>20</v>
+      </c>
+      <c r="C135" t="s">
+        <v>29</v>
+      </c>
+      <c r="D135" t="s">
+        <v>29</v>
+      </c>
+      <c r="E135" t="s">
+        <v>21</v>
+      </c>
+      <c r="F135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>45932</v>
+      </c>
+      <c r="B136">
+        <v>20</v>
+      </c>
+      <c r="C136" t="s">
+        <v>29</v>
+      </c>
+      <c r="D136" t="s">
+        <v>29</v>
+      </c>
+      <c r="E136" t="s">
+        <v>21</v>
+      </c>
+      <c r="F136">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>45933</v>
+      </c>
+      <c r="B137">
+        <v>20</v>
+      </c>
+      <c r="C137" t="s">
+        <v>29</v>
+      </c>
+      <c r="D137" t="s">
+        <v>29</v>
+      </c>
+      <c r="E137" t="s">
+        <v>21</v>
+      </c>
+      <c r="F137">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>45934</v>
+      </c>
+      <c r="B138">
+        <v>20</v>
+      </c>
+      <c r="C138" t="s">
+        <v>29</v>
+      </c>
+      <c r="D138" t="s">
+        <v>29</v>
+      </c>
+      <c r="E138" t="s">
+        <v>21</v>
+      </c>
+      <c r="F138">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>45935</v>
+      </c>
+      <c r="B139">
+        <v>20</v>
+      </c>
+      <c r="C139" t="s">
+        <v>29</v>
+      </c>
+      <c r="D139" t="s">
+        <v>29</v>
+      </c>
+      <c r="E139" t="s">
+        <v>16</v>
+      </c>
+      <c r="G139" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>45936</v>
+      </c>
+      <c r="B140">
+        <v>21</v>
+      </c>
+      <c r="C140" t="s">
+        <v>29</v>
+      </c>
+      <c r="D140" t="s">
+        <v>29</v>
+      </c>
+      <c r="E140" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>45937</v>
+      </c>
+      <c r="B141">
+        <v>21</v>
+      </c>
+      <c r="C141" t="s">
+        <v>29</v>
+      </c>
+      <c r="D141" t="s">
+        <v>29</v>
+      </c>
+      <c r="E141" t="s">
+        <v>21</v>
+      </c>
+      <c r="F141" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>45938</v>
+      </c>
+      <c r="B142">
+        <v>21</v>
+      </c>
+      <c r="C142" t="s">
+        <v>29</v>
+      </c>
+      <c r="D142" t="s">
+        <v>29</v>
+      </c>
+      <c r="E142" t="s">
+        <v>21</v>
+      </c>
+      <c r="F142">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>45939</v>
+      </c>
+      <c r="B143">
+        <v>21</v>
+      </c>
+      <c r="C143" t="s">
+        <v>29</v>
+      </c>
+      <c r="D143" t="s">
+        <v>29</v>
+      </c>
+      <c r="E143" t="s">
+        <v>21</v>
+      </c>
+      <c r="F143">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>45940</v>
+      </c>
+      <c r="B144">
+        <v>21</v>
+      </c>
+      <c r="C144" t="s">
+        <v>29</v>
+      </c>
+      <c r="D144" t="s">
+        <v>29</v>
+      </c>
+      <c r="E144" t="s">
+        <v>21</v>
+      </c>
+      <c r="F144">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>45941</v>
+      </c>
+      <c r="B145">
+        <v>21</v>
+      </c>
+      <c r="C145" t="s">
+        <v>29</v>
+      </c>
+      <c r="D145" t="s">
+        <v>29</v>
+      </c>
+      <c r="E145" t="s">
+        <v>27</v>
+      </c>
+      <c r="G145" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nuevos modelos de ML
</commit_message>
<xml_diff>
--- a/data/ref/Microciclos.xlsx
+++ b/data/ref/Microciclos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3637CD39-DC75-427A-98C4-3B668E33D53D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E227D6-180E-4990-97FA-F24D4586A67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D2A59680-2B68-43A7-A0B3-40444AC197F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="36">
   <si>
     <t>Fecha</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Pumas</t>
+  </si>
+  <si>
+    <t>Mazatlan</t>
   </si>
 </sst>
 </file>
@@ -528,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6662318-5429-45BF-A116-92A73FB7B911}">
-  <dimension ref="A1:G145"/>
+  <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="126" workbookViewId="0">
-      <selection activeCell="G146" sqref="G146"/>
+    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="126" workbookViewId="0">
+      <selection activeCell="A154" sqref="A154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,7 +542,7 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3248,6 +3251,160 @@
         <v>11</v>
       </c>
     </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>45942</v>
+      </c>
+      <c r="B146">
+        <v>21</v>
+      </c>
+      <c r="C146" t="s">
+        <v>29</v>
+      </c>
+      <c r="D146" t="s">
+        <v>29</v>
+      </c>
+      <c r="E146" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>45943</v>
+      </c>
+      <c r="B147">
+        <v>22</v>
+      </c>
+      <c r="C147" t="s">
+        <v>29</v>
+      </c>
+      <c r="D147" t="s">
+        <v>29</v>
+      </c>
+      <c r="E147" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>45944</v>
+      </c>
+      <c r="B148">
+        <v>22</v>
+      </c>
+      <c r="C148" t="s">
+        <v>29</v>
+      </c>
+      <c r="D148" t="s">
+        <v>29</v>
+      </c>
+      <c r="E148" t="s">
+        <v>21</v>
+      </c>
+      <c r="F148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>45945</v>
+      </c>
+      <c r="B149">
+        <v>22</v>
+      </c>
+      <c r="C149" t="s">
+        <v>29</v>
+      </c>
+      <c r="D149" t="s">
+        <v>29</v>
+      </c>
+      <c r="E149" t="s">
+        <v>21</v>
+      </c>
+      <c r="F149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>45946</v>
+      </c>
+      <c r="B150">
+        <v>22</v>
+      </c>
+      <c r="C150" t="s">
+        <v>29</v>
+      </c>
+      <c r="D150" t="s">
+        <v>29</v>
+      </c>
+      <c r="E150" t="s">
+        <v>21</v>
+      </c>
+      <c r="F150">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>45947</v>
+      </c>
+      <c r="B151">
+        <v>22</v>
+      </c>
+      <c r="C151" t="s">
+        <v>29</v>
+      </c>
+      <c r="D151" t="s">
+        <v>29</v>
+      </c>
+      <c r="E151" t="s">
+        <v>21</v>
+      </c>
+      <c r="F151">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>45948</v>
+      </c>
+      <c r="B152">
+        <v>22</v>
+      </c>
+      <c r="C152" t="s">
+        <v>29</v>
+      </c>
+      <c r="D152" t="s">
+        <v>29</v>
+      </c>
+      <c r="E152" t="s">
+        <v>16</v>
+      </c>
+      <c r="G152" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>45949</v>
+      </c>
+      <c r="B153">
+        <v>22</v>
+      </c>
+      <c r="C153" t="s">
+        <v>29</v>
+      </c>
+      <c r="D153" t="s">
+        <v>29</v>
+      </c>
+      <c r="E153" t="s">
+        <v>21</v>
+      </c>
+      <c r="F153">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nuevos modelos de predicción semanal
</commit_message>
<xml_diff>
--- a/data/ref/Microciclos.xlsx
+++ b/data/ref/Microciclos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03E227D6-180E-4990-97FA-F24D4586A67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EA3B2B-B860-44B4-9805-473EEE83F781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D2A59680-2B68-43A7-A0B3-40444AC197F4}"/>
   </bookViews>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6662318-5429-45BF-A116-92A73FB7B911}">
   <dimension ref="A1:G153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="126" workbookViewId="0">
-      <selection activeCell="A154" sqref="A154"/>
+    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="126" workbookViewId="0">
+      <selection activeCell="G100" sqref="G100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2375,7 +2375,7 @@
         <v>21</v>
       </c>
       <c r="F100">
-        <v>-3</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modelo de Ml predicción de Semana finalizado
</commit_message>
<xml_diff>
--- a/data/ref/Microciclos.xlsx
+++ b/data/ref/Microciclos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EA3B2B-B860-44B4-9805-473EEE83F781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1F217E-ED37-4742-B137-A1E9304408FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D2A59680-2B68-43A7-A0B3-40444AC197F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="39">
   <si>
     <t>Fecha</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Mazatlan</t>
+  </si>
+  <si>
+    <t>Queretaro</t>
+  </si>
+  <si>
+    <t>Atlas</t>
+  </si>
+  <si>
+    <t>Pachuca</t>
   </si>
 </sst>
 </file>
@@ -531,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6662318-5429-45BF-A116-92A73FB7B911}">
-  <dimension ref="A1:G153"/>
+  <dimension ref="A1:G167"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="126" workbookViewId="0">
-      <selection activeCell="G100" sqref="G100"/>
+    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="126" workbookViewId="0">
+      <selection activeCell="H165" sqref="H165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3405,6 +3414,280 @@
         <v>1</v>
       </c>
     </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>45950</v>
+      </c>
+      <c r="B154">
+        <v>23</v>
+      </c>
+      <c r="C154" t="s">
+        <v>29</v>
+      </c>
+      <c r="D154" t="s">
+        <v>29</v>
+      </c>
+      <c r="E154" t="s">
+        <v>21</v>
+      </c>
+      <c r="F154">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>45951</v>
+      </c>
+      <c r="B155">
+        <v>23</v>
+      </c>
+      <c r="C155" t="s">
+        <v>29</v>
+      </c>
+      <c r="D155" t="s">
+        <v>29</v>
+      </c>
+      <c r="E155" t="s">
+        <v>21</v>
+      </c>
+      <c r="F155">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>45952</v>
+      </c>
+      <c r="B156">
+        <v>23</v>
+      </c>
+      <c r="C156" t="s">
+        <v>29</v>
+      </c>
+      <c r="D156" t="s">
+        <v>29</v>
+      </c>
+      <c r="E156" t="s">
+        <v>16</v>
+      </c>
+      <c r="G156" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>45953</v>
+      </c>
+      <c r="B157">
+        <v>23</v>
+      </c>
+      <c r="C157" t="s">
+        <v>29</v>
+      </c>
+      <c r="D157" t="s">
+        <v>29</v>
+      </c>
+      <c r="E157" t="s">
+        <v>21</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>45954</v>
+      </c>
+      <c r="B158">
+        <v>23</v>
+      </c>
+      <c r="C158" t="s">
+        <v>29</v>
+      </c>
+      <c r="D158" t="s">
+        <v>29</v>
+      </c>
+      <c r="E158" t="s">
+        <v>21</v>
+      </c>
+      <c r="F158">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>45955</v>
+      </c>
+      <c r="B159">
+        <v>23</v>
+      </c>
+      <c r="C159" t="s">
+        <v>29</v>
+      </c>
+      <c r="D159" t="s">
+        <v>29</v>
+      </c>
+      <c r="E159" t="s">
+        <v>16</v>
+      </c>
+      <c r="G159" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>45956</v>
+      </c>
+      <c r="B160">
+        <v>23</v>
+      </c>
+      <c r="C160" t="s">
+        <v>29</v>
+      </c>
+      <c r="D160" t="s">
+        <v>29</v>
+      </c>
+      <c r="E160" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>45957</v>
+      </c>
+      <c r="B161">
+        <v>24</v>
+      </c>
+      <c r="C161" t="s">
+        <v>29</v>
+      </c>
+      <c r="D161" t="s">
+        <v>29</v>
+      </c>
+      <c r="E161" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>45958</v>
+      </c>
+      <c r="B162">
+        <v>24</v>
+      </c>
+      <c r="C162" t="s">
+        <v>29</v>
+      </c>
+      <c r="D162" t="s">
+        <v>29</v>
+      </c>
+      <c r="E162" t="s">
+        <v>21</v>
+      </c>
+      <c r="F162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>45959</v>
+      </c>
+      <c r="B163">
+        <v>24</v>
+      </c>
+      <c r="C163" t="s">
+        <v>29</v>
+      </c>
+      <c r="D163" t="s">
+        <v>29</v>
+      </c>
+      <c r="E163" t="s">
+        <v>21</v>
+      </c>
+      <c r="F163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>45960</v>
+      </c>
+      <c r="B164">
+        <v>24</v>
+      </c>
+      <c r="C164" t="s">
+        <v>29</v>
+      </c>
+      <c r="D164" t="s">
+        <v>29</v>
+      </c>
+      <c r="E164" t="s">
+        <v>21</v>
+      </c>
+      <c r="F164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>45961</v>
+      </c>
+      <c r="B165">
+        <v>24</v>
+      </c>
+      <c r="C165" t="s">
+        <v>29</v>
+      </c>
+      <c r="D165" t="s">
+        <v>29</v>
+      </c>
+      <c r="E165" t="s">
+        <v>21</v>
+      </c>
+      <c r="F165">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>45962</v>
+      </c>
+      <c r="B166">
+        <v>24</v>
+      </c>
+      <c r="C166" t="s">
+        <v>29</v>
+      </c>
+      <c r="D166" t="s">
+        <v>29</v>
+      </c>
+      <c r="E166" t="s">
+        <v>21</v>
+      </c>
+      <c r="F166">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>45963</v>
+      </c>
+      <c r="B167">
+        <v>24</v>
+      </c>
+      <c r="C167" t="s">
+        <v>29</v>
+      </c>
+      <c r="D167" t="s">
+        <v>29</v>
+      </c>
+      <c r="E167" t="s">
+        <v>16</v>
+      </c>
+      <c r="G167" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Nuevos modelos de ML en cascada
</commit_message>
<xml_diff>
--- a/data/ref/Microciclos.xlsx
+++ b/data/ref/Microciclos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nico\Desktop\DATA SCIENCE\PP- VOLUNTAREADO\chivas-ml\data\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1F217E-ED37-4742-B137-A1E9304408FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F836979B-47E8-4E86-95BB-36181EA54926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D2A59680-2B68-43A7-A0B3-40444AC197F4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="40">
   <si>
     <t>Fecha</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Pachuca</t>
+  </si>
+  <si>
+    <t>Monterrey</t>
   </si>
 </sst>
 </file>
@@ -540,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6662318-5429-45BF-A116-92A73FB7B911}">
-  <dimension ref="A1:G167"/>
+  <dimension ref="A1:G174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScale="126" workbookViewId="0">
-      <selection activeCell="H165" sqref="H165"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="126" workbookViewId="0">
+      <selection activeCell="D175" sqref="A175:D175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,6 +3691,140 @@
         <v>38</v>
       </c>
     </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>45964</v>
+      </c>
+      <c r="B168">
+        <v>25</v>
+      </c>
+      <c r="C168" t="s">
+        <v>29</v>
+      </c>
+      <c r="D168" t="s">
+        <v>29</v>
+      </c>
+      <c r="E168" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>45965</v>
+      </c>
+      <c r="B169">
+        <v>25</v>
+      </c>
+      <c r="C169" t="s">
+        <v>29</v>
+      </c>
+      <c r="D169" t="s">
+        <v>29</v>
+      </c>
+      <c r="E169" t="s">
+        <v>21</v>
+      </c>
+      <c r="F169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>45966</v>
+      </c>
+      <c r="B170">
+        <v>25</v>
+      </c>
+      <c r="C170" t="s">
+        <v>29</v>
+      </c>
+      <c r="D170" t="s">
+        <v>29</v>
+      </c>
+      <c r="E170" t="s">
+        <v>21</v>
+      </c>
+      <c r="F170">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>45967</v>
+      </c>
+      <c r="B171">
+        <v>25</v>
+      </c>
+      <c r="C171" t="s">
+        <v>29</v>
+      </c>
+      <c r="D171" t="s">
+        <v>29</v>
+      </c>
+      <c r="E171" t="s">
+        <v>21</v>
+      </c>
+      <c r="F171">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>45968</v>
+      </c>
+      <c r="B172">
+        <v>25</v>
+      </c>
+      <c r="C172" t="s">
+        <v>29</v>
+      </c>
+      <c r="D172" t="s">
+        <v>29</v>
+      </c>
+      <c r="E172" t="s">
+        <v>21</v>
+      </c>
+      <c r="F172">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>45969</v>
+      </c>
+      <c r="B173">
+        <v>25</v>
+      </c>
+      <c r="C173" t="s">
+        <v>29</v>
+      </c>
+      <c r="D173" t="s">
+        <v>29</v>
+      </c>
+      <c r="E173" t="s">
+        <v>16</v>
+      </c>
+      <c r="G173" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>45970</v>
+      </c>
+      <c r="B174">
+        <v>25</v>
+      </c>
+      <c r="C174" t="s">
+        <v>29</v>
+      </c>
+      <c r="D174" t="s">
+        <v>29</v>
+      </c>
+      <c r="E174" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>